<commit_message>
basic e-mail automation setup
</commit_message>
<xml_diff>
--- a/OverviewSheet.xlsx
+++ b/OverviewSheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juggl\OneDrive\Desktop\Bianca_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DED21978-B6A1-433F-8848-6750982C847A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46F3558F-5A55-4F56-8787-2C71CD7BD666}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5484" yWindow="1116" windowWidth="16404" windowHeight="9420" xr2:uid="{865869D4-6298-48B4-89DB-2137F5A85B3C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22080" windowHeight="13176" xr2:uid="{865869D4-6298-48B4-89DB-2137F5A85B3C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
   <si>
     <t>Nathalie Bouchard</t>
   </si>
@@ -79,16 +79,42 @@
   </si>
   <si>
     <t>Pays Tax</t>
+  </si>
+  <si>
+    <t>Bianca Saia</t>
+  </si>
+  <si>
+    <t>E-mail</t>
+  </si>
+  <si>
+    <t>Dawson</t>
+  </si>
+  <si>
+    <t>DawsonCoding@gmail.com</t>
+  </si>
+  <si>
+    <t>bianca@divanbleu.com</t>
+  </si>
+  <si>
+    <t>Rent</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -102,7 +128,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -125,11 +151,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -137,8 +175,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -451,173 +498,232 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AAFEBC3-E0EE-4661-9849-9A709F97E730}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23.88671875" customWidth="1"/>
-    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
         <v>15</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2">
+      <c r="D2" s="2">
         <v>0.5</v>
       </c>
-      <c r="D2" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="1"/>
+      <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2">
+      <c r="D3" s="2">
         <v>0.5</v>
       </c>
-      <c r="D3" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="2">
+      <c r="D4" s="2">
         <v>0.5</v>
       </c>
-      <c r="D4" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="2">
+      <c r="D5" s="2">
         <v>0.5</v>
       </c>
-      <c r="D5" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="C6" s="2">
-        <v>0.15</v>
       </c>
       <c r="D6" s="2">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E6" s="2">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="2">
+      <c r="D7" s="2">
         <v>0.4</v>
       </c>
-      <c r="D7" s="2">
+      <c r="E7" s="2">
         <v>0.1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="2">
+      <c r="D8" s="2">
         <v>0.5</v>
       </c>
-      <c r="D8" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="2">
+      <c r="D9" s="2">
         <v>0.5</v>
       </c>
-      <c r="D9" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="1"/>
+      <c r="C10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="2">
+      <c r="D10" s="2">
         <v>0.4</v>
       </c>
-      <c r="D10" s="2">
+      <c r="E10" s="2">
         <v>0.1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="2">
+      <c r="D11" s="2">
         <v>0.4</v>
       </c>
-      <c r="D11" s="2">
+      <c r="E11" s="2">
         <v>0.1</v>
       </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="4">
+        <v>1</v>
+      </c>
+      <c r="E12" s="4">
+        <v>1</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="4">
+        <v>0</v>
+      </c>
+      <c r="E13" s="4">
+        <v>0</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
made batch script more intuitive for user, added percent completed text, this is the wrong branch for these changes...
</commit_message>
<xml_diff>
--- a/OverviewSheet.xlsx
+++ b/OverviewSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juggl\OneDrive\Desktop\Bianca_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46F3558F-5A55-4F56-8787-2C71CD7BD666}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29FCD5D9-C814-4194-8273-DBAEBC983D5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22080" windowHeight="13176" xr2:uid="{865869D4-6298-48B4-89DB-2137F5A85B3C}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="16404" windowHeight="9420" xr2:uid="{865869D4-6298-48B4-89DB-2137F5A85B3C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
   <si>
     <t>Nathalie Bouchard</t>
   </si>
@@ -91,9 +91,6 @@
   </si>
   <si>
     <t>DawsonCoding@gmail.com</t>
-  </si>
-  <si>
-    <t>bianca@divanbleu.com</t>
   </si>
   <si>
     <t>Rent</t>
@@ -501,7 +498,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -519,7 +516,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C1" t="s">
         <v>15</v>
@@ -695,9 +692,7 @@
       <c r="E12" s="4">
         <v>1</v>
       </c>
-      <c r="F12" s="5" t="s">
-        <v>20</v>
-      </c>
+      <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">

</xml_diff>

<commit_message>
Updated e-mail message, added completion percentage, and removed some extra testing print statements that were hanging around
</commit_message>
<xml_diff>
--- a/OverviewSheet.xlsx
+++ b/OverviewSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juggl\OneDrive\Desktop\Bianca_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29FCD5D9-C814-4194-8273-DBAEBC983D5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CF39EA3-19F6-478C-8062-5FB5A5862C9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2304" yWindow="2304" windowWidth="16404" windowHeight="9420" xr2:uid="{865869D4-6298-48B4-89DB-2137F5A85B3C}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
   <si>
     <t>Nathalie Bouchard</t>
   </si>
@@ -498,7 +498,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -544,6 +544,9 @@
       <c r="E2" s="2">
         <v>0</v>
       </c>
+      <c r="F2" s="5" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
@@ -684,7 +687,7 @@
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D12" s="4">
         <v>1</v>

</xml_diff>

<commit_message>
Hotfix of month string, not sending blank invoices, and converting services string to lower case before checking for suivi and premier
</commit_message>
<xml_diff>
--- a/OverviewSheet.xlsx
+++ b/OverviewSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juggl\OneDrive\Desktop\Bianca_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CF39EA3-19F6-478C-8062-5FB5A5862C9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96A1EE57-4FD2-42D0-88B1-D7C40ABE15FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="16404" windowHeight="9420" xr2:uid="{865869D4-6298-48B4-89DB-2137F5A85B3C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22080" windowHeight="13176" xr2:uid="{865869D4-6298-48B4-89DB-2137F5A85B3C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="34">
   <si>
     <t>Nathalie Bouchard</t>
   </si>
@@ -94,6 +94,45 @@
   </si>
   <si>
     <t>Rent</t>
+  </si>
+  <si>
+    <t>DB Team</t>
+  </si>
+  <si>
+    <t>Anne-Marie Pelletier</t>
+  </si>
+  <si>
+    <t>Bia Krieger</t>
+  </si>
+  <si>
+    <t>Karine Lapointe</t>
+  </si>
+  <si>
+    <t>Paul Beaudry</t>
+  </si>
+  <si>
+    <t>Delphine Detour</t>
+  </si>
+  <si>
+    <t>Sylvia Galinier</t>
+  </si>
+  <si>
+    <t>Leah Brosseau</t>
+  </si>
+  <si>
+    <t>Laurence Michael</t>
+  </si>
+  <si>
+    <t>Marion Coste</t>
+  </si>
+  <si>
+    <t>Anaïs Sersoub</t>
+  </si>
+  <si>
+    <t>Genevieve Henry</t>
+  </si>
+  <si>
+    <t>Karine Yviquel</t>
   </si>
 </sst>
 </file>
@@ -164,7 +203,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -180,6 +219,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -495,23 +552,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AAFEBC3-E0EE-4661-9849-9A709F97E730}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23.88671875" customWidth="1"/>
-    <col min="2" max="2" width="4.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.109375" customWidth="1"/>
+    <col min="4" max="4" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -519,211 +576,427 @@
         <v>20</v>
       </c>
       <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
         <v>15</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="7">
+        <v>180</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="1">
+        <v>137.97</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="10">
+        <v>103.48</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+    </row>
+    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="1">
+        <v>92</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="2">
+      <c r="B6" s="13">
+        <v>300</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="2">
         <v>0.5</v>
       </c>
-      <c r="E2" s="2">
-        <v>0</v>
-      </c>
-      <c r="F2" s="5" t="s">
+      <c r="F6" s="2">
+        <v>0</v>
+      </c>
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="7">
+        <v>115</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="7">
+        <v>149.44999999999999</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="10">
+        <v>0</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="12">
+        <v>1</v>
+      </c>
+      <c r="F9" s="12">
+        <v>1</v>
+      </c>
+      <c r="G9" s="5"/>
+    </row>
+    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="1">
+        <v>172.46</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="10">
+        <v>0</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="12">
+        <v>0</v>
+      </c>
+      <c r="F11" s="12">
+        <v>0</v>
+      </c>
+      <c r="G11" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+    <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="10">
+        <v>170</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+    </row>
+    <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="10">
+        <v>195.46</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="3">
+        <v>103.5</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="6"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="3">
+        <v>80.48</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="3">
+        <v>81</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="3">
+        <v>650</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="2">
+      <c r="B18" s="11">
+        <v>700</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="14">
         <v>0.5</v>
       </c>
-      <c r="E3" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="2">
+      <c r="F18" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="11">
+        <v>310</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E19" s="14">
         <v>0.5</v>
       </c>
-      <c r="E4" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="F19" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="3">
+        <v>80.48</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="9">
+        <v>650</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E21" s="14">
+        <v>0.15</v>
+      </c>
+      <c r="F21" s="14">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="3">
+        <v>170</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="3">
+        <v>425</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="2">
+      <c r="B24" s="9">
+        <v>0</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E24" s="14">
         <v>0.5</v>
       </c>
-      <c r="E5" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="E6" s="2">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
+      <c r="F24" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="2">
+      <c r="B25" s="11">
+        <v>298.94</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E25" s="14">
         <v>0.4</v>
       </c>
-      <c r="E7" s="2">
+      <c r="F25" s="14">
         <v>0.1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="E8" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="E9" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="E10" s="2">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="E11" s="2">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="4">
-        <v>1</v>
-      </c>
-      <c r="E12" s="4">
-        <v>1</v>
-      </c>
-      <c r="F12" s="5"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="4">
-        <v>0</v>
-      </c>
-      <c r="E13" s="4">
-        <v>0</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="6"/>
-    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G25">
+    <sortCondition ref="A25"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
spreadsheets working on newer version of pandas
</commit_message>
<xml_diff>
--- a/OverviewSheet.xlsx
+++ b/OverviewSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juggl\OneDrive\Desktop\Bianca_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23EB2706-A4E5-489D-88FA-1104212A2575}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{884DE377-E68F-4D9D-8ED7-1C4D3346F3D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22080" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40935" yWindow="1935" windowWidth="16410" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
       </xcalcf:calcFeatures>
     </ext>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mhM5EjyZ20P2ZX6tOC2hT9+rZaPgA=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mgzwLTBBhT4drQim3eu7y+CF46wLQ=="/>
     </ext>
   </extLst>
 </workbook>
@@ -74,27 +74,27 @@
     <t>Anne-Marie Pelletier</t>
   </si>
   <si>
+    <t>anne-marie@divanbleu.com</t>
+  </si>
+  <si>
+    <t>Anne-Sophie Hollender</t>
+  </si>
+  <si>
+    <t>annesophie@divanbleu.com</t>
+  </si>
+  <si>
+    <t>Aurélie Olivier</t>
+  </si>
+  <si>
+    <t>aurelie@divanbleu.com</t>
+  </si>
+  <si>
+    <t>Bia Krieger</t>
+  </si>
+  <si>
     <t>N</t>
   </si>
   <si>
-    <t>Annemarie.pelletier748@gmail.com</t>
-  </si>
-  <si>
-    <t>Anne-Sophie Hollender</t>
-  </si>
-  <si>
-    <t>annesophie@divanbleu.com</t>
-  </si>
-  <si>
-    <t>Aurélie Olivier</t>
-  </si>
-  <si>
-    <t>aurelie@divanbleu.com</t>
-  </si>
-  <si>
-    <t>Bia Krieger</t>
-  </si>
-  <si>
     <t>beatris.krieger.tra@gmail.com</t>
   </si>
   <si>
@@ -110,10 +110,16 @@
     <t>christophe@divanbleu.com</t>
   </si>
   <si>
-    <t>Delphine Detour</t>
-  </si>
-  <si>
-    <t>ddeltourtra@gmail.com</t>
+    <t>Dawson</t>
+  </si>
+  <si>
+    <t>DawsonCoding@gmail.com</t>
+  </si>
+  <si>
+    <t>Delphine Deltour</t>
+  </si>
+  <si>
+    <t>delphine@divanbleu.com</t>
   </si>
   <si>
     <t>Genevieve Henry</t>
@@ -140,12 +146,6 @@
     <t>laurencemichaeli@hotmail.com</t>
   </si>
   <si>
-    <t>Leah Brosseau</t>
-  </si>
-  <si>
-    <t>lea_ballerina_inc@hotmail.com</t>
-  </si>
-  <si>
     <t>Marie-Daniel Lussier</t>
   </si>
   <si>
@@ -191,14 +191,14 @@
     <t>Marie-Josée Boivin</t>
   </si>
   <si>
-    <t>marie.j@therapielanaudiere.com</t>
+    <t>marie-josee@divanbleu.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -225,6 +225,11 @@
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0563C1"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -279,7 +284,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -297,10 +302,24 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -311,15 +330,22 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -535,10 +561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G999"/>
+  <dimension ref="A1:G998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -625,29 +651,33 @@
       <c r="A4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="6">
-        <v>164</v>
-      </c>
-      <c r="C4" s="4" t="s">
+      <c r="B4" s="7">
+        <v>250</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="F4" s="9">
+        <v>0</v>
+      </c>
+      <c r="G4" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="1" t="s">
+    </row>
+    <row r="5" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="11" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="8">
+      <c r="B5" s="12">
         <v>260.93</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="4" t="s">
@@ -659,13 +689,13 @@
       <c r="F5" s="5">
         <v>0</v>
       </c>
-      <c r="G5" s="7" t="s">
-        <v>16</v>
+      <c r="G5" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" s="2">
         <v>0</v>
@@ -683,18 +713,18 @@
         <v>0.1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="13">
+        <v>90</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="B7" s="3">
-        <v>133.25</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>8</v>
@@ -709,8 +739,8 @@
       <c r="A8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="4">
-        <v>1</v>
+      <c r="B8" s="8">
+        <v>0.01</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>8</v>
@@ -724,11 +754,11 @@
       <c r="F8" s="5">
         <v>1</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="G8" s="14" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>23</v>
       </c>
@@ -751,135 +781,145 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="8">
+        <v>0</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="5">
+        <v>0</v>
+      </c>
+      <c r="F10" s="5">
+        <v>0</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="6">
         <v>147.86000000000001</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="6">
+      <c r="C11" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="F11" s="16">
+        <v>0</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="6">
         <v>174.25</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="12">
+      <c r="C12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="18">
         <v>92.25</v>
       </c>
-      <c r="C12" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="14" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="12">
+      <c r="C13" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="21">
         <v>71.75</v>
       </c>
-      <c r="C13" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" s="12">
-        <v>71.75</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
+      <c r="C14" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
       <c r="G14" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="12">
-        <v>579.47</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>8</v>
-      </c>
+      <c r="B15" s="18">
+        <v>71.75</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
       <c r="G15" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="12">
-        <v>717.5</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E16" s="16">
+      <c r="B16" s="21">
+        <v>624.04999999999995</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="24">
         <v>0.5</v>
       </c>
-      <c r="F16" s="16">
+      <c r="F16" s="24">
         <v>0</v>
       </c>
       <c r="G16" s="1" t="s">
@@ -887,22 +927,22 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="B17" s="11">
+      <c r="B17" s="25">
         <v>150</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="17" t="s">
         <v>8</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E17" s="16">
+      <c r="E17" s="24">
         <v>0.5</v>
       </c>
-      <c r="F17" s="16">
+      <c r="F17" s="24">
         <v>0</v>
       </c>
       <c r="G17" s="1" t="s">
@@ -910,22 +950,22 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="15" t="s">
+      <c r="A18" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="B18" s="17">
+      <c r="B18" s="26">
         <v>579.47</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="C18" s="22" t="s">
         <v>8</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E18" s="16">
+      <c r="E18" s="24">
         <v>0.15</v>
       </c>
-      <c r="F18" s="16">
+      <c r="F18" s="24">
         <v>0.15</v>
       </c>
       <c r="G18" s="1" t="s">
@@ -933,14 +973,14 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="B19" s="12">
+      <c r="B19" s="18">
         <v>151.55000000000001</v>
       </c>
-      <c r="C19" s="11" t="s">
-        <v>13</v>
+      <c r="C19" s="17" t="s">
+        <v>19</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>8</v>
@@ -950,14 +990,14 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="B20" s="18">
+      <c r="B20" s="21">
         <v>225</v>
       </c>
-      <c r="C20" s="11" t="s">
-        <v>13</v>
+      <c r="C20" s="17" t="s">
+        <v>19</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>8</v>
@@ -967,22 +1007,22 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="15" t="s">
+      <c r="A21" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="B21" s="17">
+      <c r="B21" s="26">
         <v>375</v>
       </c>
-      <c r="C21" s="15" t="s">
+      <c r="C21" s="22" t="s">
         <v>8</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E21" s="16">
+      <c r="E21" s="24">
         <v>0.5</v>
       </c>
-      <c r="F21" s="16">
+      <c r="F21" s="24">
         <v>0</v>
       </c>
       <c r="G21" s="1" t="s">
@@ -990,22 +1030,22 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="11" t="s">
+      <c r="A22" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="B22" s="12">
-        <v>330</v>
-      </c>
-      <c r="C22" s="11" t="s">
+      <c r="B22" s="21">
+        <v>650</v>
+      </c>
+      <c r="C22" s="17" t="s">
         <v>8</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E22" s="16">
+      <c r="E22" s="24">
         <v>0.5</v>
       </c>
-      <c r="F22" s="16">
+      <c r="F22" s="24">
         <v>0</v>
       </c>
       <c r="G22" s="1" t="s">
@@ -1016,24 +1056,30 @@
       <c r="A23" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B23" s="19">
+      <c r="B23" s="27">
         <v>300</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>13</v>
+      <c r="C23" s="10" t="s">
+        <v>8</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G23" s="9" t="s">
+      <c r="E23" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="F23" s="10">
+        <v>0</v>
+      </c>
+      <c r="G23" s="28" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="1"/>
-    </row>
+    <row r="25" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="1"/>
+    </row>
+    <row r="26" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="28" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="29" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2006,11 +2052,9 @@
     <row r="996" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G8" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="G23" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
fixed December Rent bug
</commit_message>
<xml_diff>
--- a/OverviewSheet.xlsx
+++ b/OverviewSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juggl\OneDrive\Desktop\Bianca_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{884DE377-E68F-4D9D-8ED7-1C4D3346F3D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65E05FB5-563F-4D4A-AE1D-49ED69402C77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40935" yWindow="1935" windowWidth="16410" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22080" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="51">
   <si>
     <t>Name</t>
   </si>
@@ -108,12 +108,6 @@
   </si>
   <si>
     <t>christophe@divanbleu.com</t>
-  </si>
-  <si>
-    <t>Dawson</t>
-  </si>
-  <si>
-    <t>DawsonCoding@gmail.com</t>
   </si>
   <si>
     <t>Delphine Deltour</t>
@@ -561,10 +555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G998"/>
+  <dimension ref="A1:G997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -782,67 +776,63 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10" s="6">
+        <v>147.86000000000001</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="F10" s="16">
         <v>0</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="G10" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="6">
+        <v>174.25</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="5">
-        <v>0</v>
-      </c>
-      <c r="F10" s="5">
-        <v>0</v>
-      </c>
-      <c r="G10" s="11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="6">
-        <v>147.86000000000001</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>8</v>
-      </c>
       <c r="D11" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="16">
-        <v>0.5</v>
-      </c>
-      <c r="F11" s="16">
-        <v>0</v>
-      </c>
-      <c r="G11" s="10" t="s">
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="6">
-        <v>174.25</v>
-      </c>
-      <c r="C12" s="4" t="s">
+      <c r="B12" s="18">
+        <v>92.25</v>
+      </c>
+      <c r="C12" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="1" t="s">
+      <c r="D12" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="20" t="s">
         <v>30</v>
       </c>
     </row>
@@ -850,18 +840,18 @@
       <c r="A13" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="18">
-        <v>92.25</v>
+      <c r="B13" s="21">
+        <v>71.75</v>
       </c>
       <c r="C13" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="20" t="s">
+      <c r="D13" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="1" t="s">
         <v>32</v>
       </c>
     </row>
@@ -869,7 +859,7 @@
       <c r="A14" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="21">
+      <c r="B14" s="18">
         <v>71.75</v>
       </c>
       <c r="C14" s="17" t="s">
@@ -888,17 +878,21 @@
       <c r="A15" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="18">
-        <v>71.75</v>
+      <c r="B15" s="21">
+        <v>624.04999999999995</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
+        <v>8</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="F15" s="24">
+        <v>0</v>
+      </c>
       <c r="G15" s="1" t="s">
         <v>36</v>
       </c>
@@ -907,13 +901,13 @@
       <c r="A16" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="21">
-        <v>624.04999999999995</v>
+      <c r="B16" s="25">
+        <v>150</v>
       </c>
       <c r="C16" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="23" t="s">
+      <c r="D16" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E16" s="24">
@@ -927,46 +921,40 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="B17" s="25">
-        <v>150</v>
-      </c>
-      <c r="C17" s="17" t="s">
+      <c r="B17" s="26">
+        <v>579.47</v>
+      </c>
+      <c r="C17" s="22" t="s">
         <v>8</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E17" s="24">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="F17" s="24">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="22" t="s">
+      <c r="A18" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="B18" s="26">
-        <v>579.47</v>
-      </c>
-      <c r="C18" s="22" t="s">
-        <v>8</v>
+      <c r="B18" s="18">
+        <v>151.55000000000001</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>19</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="E18" s="24">
-        <v>0.15</v>
-      </c>
-      <c r="F18" s="24">
-        <v>0.15</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>42</v>
@@ -976,8 +964,8 @@
       <c r="A19" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="B19" s="18">
-        <v>151.55000000000001</v>
+      <c r="B19" s="21">
+        <v>225</v>
       </c>
       <c r="C19" s="17" t="s">
         <v>19</v>
@@ -990,30 +978,36 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="17" t="s">
+      <c r="A20" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="B20" s="21">
-        <v>225</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>19</v>
+      <c r="B20" s="26">
+        <v>375</v>
+      </c>
+      <c r="C20" s="22" t="s">
+        <v>8</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="E20" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="F20" s="24">
+        <v>0</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="22" t="s">
+      <c r="A21" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="B21" s="26">
-        <v>375</v>
-      </c>
-      <c r="C21" s="22" t="s">
+      <c r="B21" s="21">
+        <v>650</v>
+      </c>
+      <c r="C21" s="17" t="s">
         <v>8</v>
       </c>
       <c r="D21" s="2" t="s">
@@ -1030,55 +1024,33 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="17" t="s">
+      <c r="A22" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B22" s="21">
-        <v>650</v>
-      </c>
-      <c r="C22" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E22" s="24">
+      <c r="B22" s="27">
+        <v>300</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="10">
         <v>0.5</v>
       </c>
-      <c r="F22" s="24">
+      <c r="F22" s="10">
         <v>0</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="G22" s="28" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B23" s="27">
-        <v>300</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E23" s="10">
-        <v>0.5</v>
-      </c>
-      <c r="F23" s="10">
-        <v>0</v>
-      </c>
-      <c r="G23" s="28" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="1"/>
-    </row>
+    <row r="23" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="1"/>
+    </row>
+    <row r="25" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="26" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="28" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2051,7 +2023,6 @@
     <row r="995" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="996" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G8" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>